<commit_message>
trabajando con cp imposicion
</commit_message>
<xml_diff>
--- a/inclusion cortito.xlsx
+++ b/inclusion cortito.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$H$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$H$3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>pesoenvio</t>
   </si>
@@ -30,30 +30,9 @@
     <t>0.25</t>
   </si>
   <si>
-    <t>ROSARIO</t>
-  </si>
-  <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>RIOJA 1474</t>
-  </si>
-  <si>
-    <t>REGINA TRIPALDI</t>
-  </si>
-  <si>
-    <t>MENDOZA 3386</t>
-  </si>
-  <si>
-    <t>RECEPCIONISTA ESTUDIO CASIELLO</t>
-  </si>
-  <si>
-    <t>1.34</t>
-  </si>
-  <si>
-    <t>2.3</t>
-  </si>
-  <si>
     <t>PRODUCTO</t>
   </si>
   <si>
@@ -91,6 +70,12 @@
   </si>
   <si>
     <t>rosarió</t>
+  </si>
+  <si>
+    <t>2817290183012</t>
+  </si>
+  <si>
+    <t>2818101030312</t>
   </si>
 </sst>
 </file>
@@ -151,11 +136,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -167,6 +149,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -449,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -457,121 +446,81 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="12.5703125" style="4"/>
+    <col min="1" max="1" width="25.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="12.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>16</v>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>28172901830</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3">
         <v>2000</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>3</v>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>28181010303</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="A3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3">
         <v>2000</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>28182788096</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2000</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>28190726094</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2000</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ahora sirve para cualquier sucursal
</commit_message>
<xml_diff>
--- a/inclusion cortito.xlsx
+++ b/inclusion cortito.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>pesoenvio</t>
   </si>
@@ -438,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="3">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>2</v>
@@ -517,9 +517,49 @@
         <v>15</v>
       </c>
       <c r="E3" s="3">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5000</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>